<commit_message>
added fisher cat for daniel smith
</commit_message>
<xml_diff>
--- a/2019BIO2029/DanielSmith_C300.xlsx
+++ b/2019BIO2029/DanielSmith_C300.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="76">
   <si>
     <t xml:space="preserve">Wildcard </t>
   </si>
@@ -685,8 +685,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="P20" sqref="P20"/>
+    <sheetView tabSelected="1" topLeftCell="H13" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1189,7 +1189,9 @@
       <c r="D24" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="L24" s="3"/>
+      <c r="L24" s="3" t="s">
+        <v>60</v>
+      </c>
       <c r="N24" s="9" t="s">
         <v>59</v>
       </c>

</xml_diff>